<commit_message>
Atualização do controle de artigos científicos
</commit_message>
<xml_diff>
--- a/Bibliografia/Listagem.xlsx
+++ b/Bibliografia/Listagem.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27a8628a50772066/R/ICSAP/Bibliografia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="913" documentId="8_{A970F4A6-B25B-4E0A-B438-2B0FA64B278E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{383514E2-8CAA-42C6-801C-EDE9C00BBB55}"/>
+  <xr:revisionPtr revIDLastSave="940" documentId="8_{A970F4A6-B25B-4E0A-B438-2B0FA64B278E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{113B0C79-B131-4440-AE92-6A98EE23B813}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{92966055-116D-42DB-900B-B75A724BA527}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3425" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3434" uniqueCount="341">
   <si>
     <t>Palavra-chave</t>
   </si>
@@ -1113,6 +1113,17 @@
 3) Teste post hoc de Dunnett
 4) Correlação (Spearman)
 5) Razão de taxas</t>
+  </si>
+  <si>
+    <t>1) Análise descritiva
+2) Correlação linear</t>
+  </si>
+  <si>
+    <t>1) Regressão linear</t>
+  </si>
+  <si>
+    <t>1) Estatística descritiva
+2) Correlação de Spearman</t>
   </si>
 </sst>
 </file>
@@ -1607,12 +1618,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE712DB-CC69-4EE6-896B-656C736DF159}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:L227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1670,7 +1680,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>21</v>
       </c>
@@ -1699,9 +1709,11 @@
       <c r="J2" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="K2" s="15"/>
-    </row>
-    <row r="3" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K2" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>25</v>
       </c>
@@ -1737,7 +1749,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
@@ -1768,7 +1780,7 @@
       </c>
       <c r="K4" s="15"/>
     </row>
-    <row r="5" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>240</v>
       </c>
@@ -1806,7 +1818,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>72</v>
       </c>
@@ -1844,7 +1856,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>67</v>
       </c>
@@ -1946,7 +1958,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -1984,7 +1996,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="120" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="120" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>55</v>
       </c>
@@ -2020,7 +2032,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>78</v>
       </c>
@@ -2045,13 +2057,20 @@
       <c r="H12" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="I12" s="16"/>
+      <c r="I12" s="16" t="s">
+        <v>339</v>
+      </c>
       <c r="J12" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="K12" s="15"/>
-    </row>
-    <row r="13" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K12" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>256</v>
       </c>
@@ -2087,7 +2106,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>35</v>
       </c>
@@ -2118,7 +2137,7 @@
       </c>
       <c r="K14" s="15"/>
     </row>
-    <row r="15" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>236</v>
       </c>
@@ -2143,10 +2162,18 @@
       <c r="H15" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="I15" s="16"/>
+      <c r="I15" s="16" t="s">
+        <v>340</v>
+      </c>
       <c r="J15" s="18"/>
-    </row>
-    <row r="16" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K15" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="L15" s="18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>121</v>
       </c>
@@ -2177,7 +2204,7 @@
       </c>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>62</v>
       </c>
@@ -2213,7 +2240,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="72" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>7</v>
       </c>
@@ -2282,7 +2309,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>243</v>
       </c>
@@ -2310,7 +2337,7 @@
       <c r="I20" s="16"/>
       <c r="J20" s="18"/>
     </row>
-    <row r="21" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>91</v>
       </c>
@@ -2348,7 +2375,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>100</v>
       </c>
@@ -2379,7 +2406,7 @@
       </c>
       <c r="K22" s="15"/>
     </row>
-    <row r="23" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>88</v>
       </c>
@@ -2417,7 +2444,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>105</v>
       </c>
@@ -2448,7 +2475,7 @@
       </c>
       <c r="K24" s="15"/>
     </row>
-    <row r="25" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>29</v>
       </c>
@@ -2486,7 +2513,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>113</v>
       </c>
@@ -2517,7 +2544,7 @@
       </c>
       <c r="K26" s="15"/>
     </row>
-    <row r="27" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>96</v>
       </c>
@@ -2548,7 +2575,7 @@
       </c>
       <c r="K27" s="15"/>
     </row>
-    <row r="28" spans="1:12" ht="108" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="108" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>126</v>
       </c>
@@ -2584,7 +2611,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>118</v>
       </c>
@@ -2640,13 +2667,18 @@
       <c r="H30" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="I30" s="16"/>
+      <c r="I30" s="16" t="s">
+        <v>338</v>
+      </c>
       <c r="J30" s="18"/>
       <c r="K30" s="18" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L30" s="18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>264</v>
       </c>
@@ -2744,7 +2776,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="36" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>281</v>
       </c>
@@ -2772,7 +2804,7 @@
       <c r="I34" s="16"/>
       <c r="J34" s="18"/>
     </row>
-    <row r="35" spans="1:11" ht="96" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="96" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>288</v>
       </c>
@@ -2800,7 +2832,7 @@
       <c r="I35" s="16"/>
       <c r="J35" s="18"/>
     </row>
-    <row r="36" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>294</v>
       </c>
@@ -2828,7 +2860,7 @@
       <c r="I36" s="16"/>
       <c r="J36" s="18"/>
     </row>
-    <row r="37" spans="1:11" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="36" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>306</v>
       </c>
@@ -2856,7 +2888,7 @@
       <c r="I37" s="16"/>
       <c r="J37" s="18"/>
     </row>
-    <row r="38" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>314</v>
       </c>
@@ -2884,7 +2916,7 @@
       <c r="I38" s="16"/>
       <c r="J38" s="18"/>
     </row>
-    <row r="39" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>321</v>
       </c>
@@ -5169,16 +5201,7 @@
       <c r="J227" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L39" xr:uid="{B3F1C4F4-92F8-4D45-9CD2-F8D7A5E8BEF7}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="A2"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="11">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L39" xr:uid="{B3F1C4F4-92F8-4D45-9CD2-F8D7A5E8BEF7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K227">
     <sortCondition ref="A2:A227"/>
   </sortState>

</xml_diff>

<commit_message>
Atualização do arquivo com as apresentações de 2021 04 07
</commit_message>
<xml_diff>
--- a/Bibliografia/Listagem.xlsx
+++ b/Bibliografia/Listagem.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27a8628a50772066/R/ICSAP/Bibliografia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="940" documentId="8_{A970F4A6-B25B-4E0A-B438-2B0FA64B278E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{113B0C79-B131-4440-AE92-6A98EE23B813}"/>
+  <xr:revisionPtr revIDLastSave="974" documentId="8_{A970F4A6-B25B-4E0A-B438-2B0FA64B278E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A4AD7CD2-1312-40FD-832C-AFD00229568E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{92966055-116D-42DB-900B-B75A724BA527}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3434" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3442" uniqueCount="344">
   <si>
     <t>Palavra-chave</t>
   </si>
@@ -1124,6 +1124,23 @@
   <si>
     <t>1) Estatística descritiva
 2) Correlação de Spearman</t>
+  </si>
+  <si>
+    <t>Revista Epidemiologia e Serviços de Saúde</t>
+  </si>
+  <si>
+    <t>1) Estatística descritiva
+2) Teste Qui-Quadrado
+3) Regressão de Poisson
+4) Regressão Binomial Negativa
+5) Imputação múltipla
+6) Razão de taxas</t>
+  </si>
+  <si>
+    <t>1) Regressão de Poisson
+2) Regressão Binomial Negativa
+3) Razão de médias
+4) Coeficiente de correlação de Spearman</t>
   </si>
 </sst>
 </file>
@@ -1621,8 +1638,8 @@
   <dimension ref="A1:L227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1925,7 +1942,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="84" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>82</v>
       </c>
@@ -1950,12 +1967,17 @@
       <c r="H9" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="I9" s="16"/>
+      <c r="I9" s="16" t="s">
+        <v>342</v>
+      </c>
       <c r="J9" s="18" t="s">
         <v>46</v>
       </c>
       <c r="K9" s="18" t="s">
         <v>134</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.2">
@@ -2452,10 +2474,10 @@
         <v>106</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>12</v>
+        <v>341</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E24" s="16" t="s">
         <v>107</v>
@@ -2469,11 +2491,18 @@
       <c r="H24" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I24" s="16"/>
+      <c r="I24" s="16" t="s">
+        <v>327</v>
+      </c>
       <c r="J24" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="K24" s="15"/>
+      <c r="K24" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="L24" s="18" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="25" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
@@ -2611,7 +2640,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="72" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>118</v>
       </c>
@@ -2636,11 +2665,18 @@
       <c r="H29" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I29" s="16"/>
+      <c r="I29" s="16" t="s">
+        <v>343</v>
+      </c>
       <c r="J29" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="K29" s="15"/>
+      <c r="K29" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="L29" s="18" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">

</xml_diff>

<commit_message>
Atualização da planilha de controle
</commit_message>
<xml_diff>
--- a/Bibliografia/Listagem.xlsx
+++ b/Bibliografia/Listagem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27a8628a50772066/R/ICSAP/Bibliografia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="974" documentId="8_{A970F4A6-B25B-4E0A-B438-2B0FA64B278E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A4AD7CD2-1312-40FD-832C-AFD00229568E}"/>
+  <xr:revisionPtr revIDLastSave="980" documentId="8_{A970F4A6-B25B-4E0A-B438-2B0FA64B278E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7B4C5F94-B777-4011-A4F6-A8C4F7014C5C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{92966055-116D-42DB-900B-B75A724BA527}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3442" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3446" uniqueCount="346">
   <si>
     <t>Palavra-chave</t>
   </si>
@@ -1141,6 +1141,13 @@
 2) Regressão Binomial Negativa
 3) Razão de médias
 4) Coeficiente de correlação de Spearman</t>
+  </si>
+  <si>
+    <t>1) Estatística descritiva</t>
+  </si>
+  <si>
+    <t>1) Razão de coeficientes
+2) Padronização de coeficientes e Razão de Morbidade Esperada (RMI)</t>
   </si>
 </sst>
 </file>
@@ -1635,11 +1642,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE712DB-CC69-4EE6-896B-656C736DF159}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1730,7 +1738,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>25</v>
       </c>
@@ -1797,7 +1805,7 @@
       </c>
       <c r="K4" s="15"/>
     </row>
-    <row r="5" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>240</v>
       </c>
@@ -1835,7 +1843,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>72</v>
       </c>
@@ -1873,7 +1881,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>67</v>
       </c>
@@ -1942,7 +1950,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="84" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="84" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>82</v>
       </c>
@@ -1980,7 +1988,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -2018,7 +2026,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="120" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="120" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>55</v>
       </c>
@@ -2054,7 +2062,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>78</v>
       </c>
@@ -2092,7 +2100,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>256</v>
       </c>
@@ -2159,7 +2167,7 @@
       </c>
       <c r="K14" s="15"/>
     </row>
-    <row r="15" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>236</v>
       </c>
@@ -2226,7 +2234,7 @@
       </c>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:12" ht="36" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>62</v>
       </c>
@@ -2262,7 +2270,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="72" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>7</v>
       </c>
@@ -2359,7 +2367,7 @@
       <c r="I20" s="16"/>
       <c r="J20" s="18"/>
     </row>
-    <row r="21" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>91</v>
       </c>
@@ -2428,7 +2436,7 @@
       </c>
       <c r="K22" s="15"/>
     </row>
-    <row r="23" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>88</v>
       </c>
@@ -2466,7 +2474,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="36" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>105</v>
       </c>
@@ -2504,7 +2512,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>29</v>
       </c>
@@ -2604,7 +2612,7 @@
       </c>
       <c r="K27" s="15"/>
     </row>
-    <row r="28" spans="1:12" ht="108" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="108" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>126</v>
       </c>
@@ -2640,7 +2648,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="72" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>118</v>
       </c>
@@ -2678,7 +2686,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>261</v>
       </c>
@@ -2714,7 +2722,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="36" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>264</v>
       </c>
@@ -2896,7 +2904,7 @@
       <c r="I36" s="16"/>
       <c r="J36" s="18"/>
     </row>
-    <row r="37" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>306</v>
       </c>
@@ -2921,8 +2929,13 @@
       <c r="H37" s="17" t="s">
         <v>304</v>
       </c>
-      <c r="I37" s="16"/>
+      <c r="I37" s="16" t="s">
+        <v>345</v>
+      </c>
       <c r="J37" s="18"/>
+      <c r="K37" s="18" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="38" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
@@ -2949,8 +2962,13 @@
       <c r="H38" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I38" s="16"/>
+      <c r="I38" s="16" t="s">
+        <v>344</v>
+      </c>
       <c r="J38" s="18"/>
+      <c r="K38" s="18" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
@@ -5237,7 +5255,11 @@
       <c r="J227" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L39" xr:uid="{B3F1C4F4-92F8-4D45-9CD2-F8D7A5E8BEF7}"/>
+  <autoFilter ref="A1:L39" xr:uid="{B3F1C4F4-92F8-4D45-9CD2-F8D7A5E8BEF7}">
+    <filterColumn colId="11">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K227">
     <sortCondition ref="A2:A227"/>
   </sortState>

</xml_diff>

<commit_message>
Arquivos removidos de local e atualizados
</commit_message>
<xml_diff>
--- a/Bibliografia/Listagem.xlsx
+++ b/Bibliografia/Listagem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27a8628a50772066/R/ICSAP/Bibliografia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="999" documentId="8_{A970F4A6-B25B-4E0A-B438-2B0FA64B278E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CDFFF870-8785-4B2B-9B40-9835F45CE735}"/>
+  <xr:revisionPtr revIDLastSave="1018" documentId="8_{A970F4A6-B25B-4E0A-B438-2B0FA64B278E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{05BE068A-45F9-4D5B-8BFA-56BF6A9187CA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{92966055-116D-42DB-900B-B75A724BA527}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3453" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3456" uniqueCount="350">
   <si>
     <t>Palavra-chave</t>
   </si>
@@ -1156,6 +1156,13 @@
   <si>
     <t>1) Regressão linear simples
 2) Coeficiente de correlação de Pearson</t>
+  </si>
+  <si>
+    <t>35 a 74 anos</t>
+  </si>
+  <si>
+    <t>1) Correlação de Pearson
+2) Correlação de Spearman</t>
   </si>
 </sst>
 </file>
@@ -1654,8 +1661,8 @@
   <dimension ref="A1:L227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1713,18 +1720,18 @@
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>14</v>
@@ -1738,199 +1745,192 @@
       <c r="H2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="16"/>
+      <c r="I2" s="16" t="s">
+        <v>336</v>
+      </c>
       <c r="J2" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="K2" s="18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K2" s="15"/>
+      <c r="L2" s="18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>28</v>
+        <v>153</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K3" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="L3" s="18" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>45</v>
+      <c r="E4" s="17" t="s">
+        <v>28</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="I4" s="16"/>
       <c r="J4" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="K4" s="15"/>
-    </row>
-    <row r="5" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>240</v>
+        <v>270</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>241</v>
+        <v>271</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>144</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>30</v>
+        <v>272</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>120</v>
+        <v>273</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>242</v>
+        <v>274</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>328</v>
-      </c>
-      <c r="J5" s="18" t="s">
-        <v>46</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="I5" s="16"/>
+      <c r="J5" s="18"/>
       <c r="K5" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>72</v>
+        <v>276</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>76</v>
+        <v>277</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>144</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>73</v>
+        <v>278</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>74</v>
+        <v>279</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>75</v>
+        <v>280</v>
       </c>
       <c r="H6" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="16" t="s">
-        <v>333</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>47</v>
-      </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="18"/>
       <c r="K6" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="L6" s="18" t="s">
-        <v>330</v>
-      </c>
     </row>
     <row r="7" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>67</v>
+      <c r="A7" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>30</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="16"/>
+        <v>33</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>331</v>
+      </c>
       <c r="J7" s="18" t="s">
         <v>46</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="L7" s="18" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>109</v>
+        <v>256</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>110</v>
+        <v>257</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>85</v>
@@ -1939,31 +1939,34 @@
         <v>144</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>107</v>
+        <v>258</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>112</v>
+        <v>259</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>111</v>
+        <v>260</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="18" t="s">
-        <v>47</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="J8" s="18"/>
       <c r="K8" s="18" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="84" hidden="1" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>82</v>
+        <v>240</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>86</v>
+        <v>241</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>85</v>
@@ -1975,107 +1978,95 @@
         <v>30</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>87</v>
+        <v>242</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="J9" s="18" t="s">
         <v>46</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L9" s="18" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>327</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="I10" s="16"/>
       <c r="J10" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="K10" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="L10" s="18" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="120" hidden="1" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>245</v>
+        <v>49</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>149</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K11" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="L11" s="18" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>12</v>
@@ -2084,124 +2075,129 @@
         <v>149</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L12" s="18" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="120" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>256</v>
+        <v>55</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>258</v>
+        <v>56</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>259</v>
+        <v>57</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>260</v>
+        <v>59</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>325</v>
-      </c>
-      <c r="J13" s="18"/>
+        <v>60</v>
+      </c>
+      <c r="I13" s="16"/>
+      <c r="J13" s="18" t="s">
+        <v>48</v>
+      </c>
       <c r="K13" s="18" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L13" s="18" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="36" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>35</v>
+        <v>243</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>41</v>
+        <v>244</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>40</v>
+        <v>246</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>37</v>
+        <v>249</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>39</v>
+        <v>250</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>38</v>
+        <v>251</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="I14" s="16"/>
-      <c r="J14" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="K14" s="15"/>
-    </row>
-    <row r="15" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+        <v>348</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>349</v>
+      </c>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>236</v>
+        <v>264</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>237</v>
+        <v>265</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>92</v>
+        <v>266</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>238</v>
+        <v>267</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>239</v>
+        <v>268</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>33</v>
+        <v>269</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="J15" s="18"/>
       <c r="K15" s="18" t="s">
@@ -2211,308 +2207,335 @@
         <v>330</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="48" x14ac:dyDescent="0.2">
-      <c r="A16" s="14" t="s">
-        <v>121</v>
+    <row r="16" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>124</v>
+        <v>69</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>125</v>
+        <v>70</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>123</v>
+        <v>30</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="H16" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I16" s="16"/>
       <c r="J16" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="K16" s="15"/>
-    </row>
-    <row r="17" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="L16" s="18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="H17" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K17" s="15"/>
+        <v>47</v>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>132</v>
+      </c>
       <c r="L17" s="18" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>7</v>
+        <v>306</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>10</v>
+        <v>304</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>12</v>
+        <v>307</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>14</v>
+        <v>305</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>16</v>
+        <v>312</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>24</v>
+        <v>313</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>20</v>
+        <v>304</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>336</v>
-      </c>
-      <c r="J18" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K18" s="15"/>
+        <v>345</v>
+      </c>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18" t="s">
+        <v>132</v>
+      </c>
       <c r="L18" s="18" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="84" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
-        <v>252</v>
+        <v>82</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>254</v>
+        <v>86</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>144</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>92</v>
+        <v>30</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>253</v>
+        <v>83</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>255</v>
+        <v>87</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>337</v>
-      </c>
-      <c r="J19" s="18"/>
+        <v>342</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>46</v>
+      </c>
       <c r="K19" s="18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="36" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="L19" s="18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>243</v>
+        <v>88</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>244</v>
+        <v>136</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>246</v>
+        <v>70</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>249</v>
+        <v>30</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>250</v>
+        <v>89</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>251</v>
+        <v>27</v>
       </c>
       <c r="H20" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I20" s="16"/>
-      <c r="J20" s="18"/>
-    </row>
-    <row r="21" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I20" s="16" t="s">
+        <v>326</v>
+      </c>
+      <c r="J20" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K20" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="L20" s="18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>90</v>
+        <v>12</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K21" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L21" s="18" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C22" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>332</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K22" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="L22" s="18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D23" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="E22" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="I22" s="16"/>
-      <c r="J22" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="K22" s="15"/>
-    </row>
-    <row r="23" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>157</v>
-      </c>
       <c r="E23" s="16" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="H23" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>326</v>
+        <v>346</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K23" s="18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="L23" s="18" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
-        <v>105</v>
+        <v>236</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>106</v>
+        <v>237</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>341</v>
+        <v>31</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>98</v>
+        <v>238</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>108</v>
+        <v>239</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>327</v>
-      </c>
-      <c r="J24" s="18" t="s">
-        <v>47</v>
-      </c>
+        <v>340</v>
+      </c>
+      <c r="J24" s="18"/>
       <c r="K24" s="18" t="s">
         <v>132</v>
       </c>
@@ -2520,81 +2543,73 @@
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
-        <v>29</v>
+        <v>252</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>30</v>
+        <v>254</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>32</v>
+        <v>253</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>34</v>
+        <v>255</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>331</v>
-      </c>
-      <c r="J25" s="18" t="s">
-        <v>46</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="J25" s="18"/>
       <c r="K25" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="L25" s="18" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="96" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
-        <v>113</v>
+        <v>288</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>117</v>
+        <v>289</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>12</v>
+        <v>290</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>114</v>
+        <v>16</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>116</v>
+        <v>293</v>
       </c>
       <c r="H26" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I26" s="16"/>
-      <c r="J26" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="K26" s="15"/>
-    </row>
-    <row r="27" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J26" s="18"/>
+    </row>
+    <row r="27" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>12</v>
@@ -2603,93 +2618,78 @@
         <v>149</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I27" s="16" t="s">
-        <v>346</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="I27" s="16"/>
       <c r="J27" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K27" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="L27" s="18" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="108" hidden="1" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="K27" s="15"/>
+    </row>
+    <row r="28" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
-        <v>126</v>
+        <v>281</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>130</v>
+        <v>282</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>12</v>
+        <v>283</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>127</v>
+        <v>30</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>128</v>
+        <v>287</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>129</v>
+        <v>286</v>
       </c>
       <c r="H28" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I28" s="16"/>
-      <c r="J28" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="K28" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="L28" s="18" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J28" s="18"/>
+    </row>
+    <row r="29" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>12</v>
+        <v>341</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="H29" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="J29" s="18" t="s">
         <v>47</v>
@@ -2701,12 +2701,12 @@
         <v>330</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
-        <v>261</v>
+        <v>109</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>262</v>
+        <v>110</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>85</v>
@@ -2715,314 +2715,329 @@
         <v>144</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>262</v>
+        <v>107</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>253</v>
+        <v>112</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>263</v>
+        <v>111</v>
       </c>
       <c r="H30" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="I30" s="16" t="s">
-        <v>338</v>
-      </c>
-      <c r="J30" s="18"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="18" t="s">
+        <v>47</v>
+      </c>
       <c r="K30" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="L30" s="18" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
-        <v>264</v>
+        <v>321</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>265</v>
+        <v>323</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>90</v>
+        <v>324</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>144</v>
+        <v>28</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>266</v>
+        <v>107</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>267</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>268</v>
+        <v>322</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>28</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>269</v>
-      </c>
-      <c r="I31" s="16" t="s">
-        <v>334</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I31" s="16"/>
       <c r="J31" s="18"/>
-      <c r="K31" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="L31" s="18" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>144</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>275</v>
-      </c>
-      <c r="I32" s="16"/>
+        <v>84</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>338</v>
+      </c>
       <c r="J32" s="18"/>
       <c r="K32" s="18" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="24" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+      <c r="L32" s="18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
-        <v>276</v>
+        <v>314</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>277</v>
+        <v>315</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>90</v>
+        <v>316</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>144</v>
+        <v>180</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>278</v>
+        <v>319</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>279</v>
+        <v>65</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>280</v>
+        <v>320</v>
       </c>
       <c r="H33" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I33" s="16"/>
+      <c r="I33" s="16" t="s">
+        <v>344</v>
+      </c>
       <c r="J33" s="18"/>
       <c r="K33" s="18" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" ht="36" x14ac:dyDescent="0.2">
+      <c r="L33" s="18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
-        <v>281</v>
+        <v>113</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>282</v>
+        <v>117</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>283</v>
+        <v>12</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>287</v>
+        <v>114</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>286</v>
+        <v>116</v>
       </c>
       <c r="H34" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I34" s="16"/>
-      <c r="J34" s="18"/>
-    </row>
-    <row r="35" spans="1:12" ht="96" x14ac:dyDescent="0.2">
+      <c r="J34" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="K34" s="15"/>
+    </row>
+    <row r="35" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
-        <v>288</v>
+        <v>118</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>289</v>
+        <v>119</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>290</v>
+        <v>12</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>16</v>
+        <v>120</v>
       </c>
       <c r="G35" s="14" t="s">
-        <v>293</v>
+        <v>115</v>
       </c>
       <c r="H35" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I35" s="16"/>
-      <c r="J35" s="18"/>
-    </row>
-    <row r="36" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+      <c r="I35" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="J35" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="K35" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="L35" s="18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
-        <v>294</v>
+        <v>121</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>298</v>
+        <v>124</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>299</v>
+        <v>125</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>296</v>
+        <v>123</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>295</v>
+        <v>122</v>
       </c>
       <c r="G36" s="14" t="s">
-        <v>297</v>
+        <v>43</v>
       </c>
       <c r="H36" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I36" s="16" t="s">
-        <v>347</v>
-      </c>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I36" s="16"/>
+      <c r="J36" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="K36" s="15"/>
+    </row>
+    <row r="37" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
-        <v>306</v>
+        <v>62</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>304</v>
+        <v>63</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>307</v>
+        <v>12</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>305</v>
+        <v>64</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>312</v>
+        <v>65</v>
       </c>
       <c r="G37" s="14" t="s">
-        <v>313</v>
+        <v>66</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>304</v>
+        <v>20</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>345</v>
-      </c>
-      <c r="J37" s="18"/>
-      <c r="K37" s="18" t="s">
-        <v>132</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="J37" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K37" s="15"/>
       <c r="L37" s="18" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>316</v>
+        <v>299</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>180</v>
+        <v>149</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>319</v>
+        <v>296</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>65</v>
+        <v>295</v>
       </c>
       <c r="G38" s="14" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="H38" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="J38" s="18"/>
       <c r="K38" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="L38" s="18" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:12" ht="108" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
-        <v>321</v>
+        <v>126</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>323</v>
+        <v>130</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>324</v>
+        <v>12</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>28</v>
+        <v>149</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>322</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>28</v>
+        <v>128</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>129</v>
       </c>
       <c r="H39" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I39" s="16"/>
-      <c r="J39" s="18"/>
+      <c r="J39" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K39" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="L39" s="18" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="14"/>
@@ -5286,8 +5301,8 @@
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K227">
-    <sortCondition ref="A2:A227"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L39">
+    <sortCondition ref="B2:B39"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização de bbibliografia e apresentações
</commit_message>
<xml_diff>
--- a/Bibliografia/Listagem.xlsx
+++ b/Bibliografia/Listagem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27a8628a50772066/R/ICSAP/Bibliografia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1022" documentId="8_{A970F4A6-B25B-4E0A-B438-2B0FA64B278E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A9EB50E3-EBE3-4551-8459-1C172DEDF95D}"/>
+  <xr:revisionPtr revIDLastSave="1027" documentId="8_{A970F4A6-B25B-4E0A-B438-2B0FA64B278E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{58FB0887-6789-4870-97B5-931B877BBD1A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{92966055-116D-42DB-900B-B75A724BA527}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3458" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3459" uniqueCount="350">
   <si>
     <t>Palavra-chave</t>
   </si>
@@ -1163,10 +1163,6 @@
   <si>
     <t>1) Correlação de Pearson
 2) Correlação de Spearman</t>
-  </si>
-  <si>
-    <t>1) Estatística descritiva
-2) Correlação</t>
   </si>
 </sst>
 </file>
@@ -1661,12 +1657,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE712DB-CC69-4EE6-896B-656C736DF159}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:L227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1724,7 +1719,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="72" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>7</v>
       </c>
@@ -1793,7 +1788,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>25</v>
       </c>
@@ -1891,7 +1886,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>29</v>
       </c>
@@ -1929,7 +1924,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>256</v>
       </c>
@@ -1965,7 +1960,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>240</v>
       </c>
@@ -2065,7 +2060,7 @@
       </c>
       <c r="K11" s="15"/>
     </row>
-    <row r="12" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>50</v>
       </c>
@@ -2103,7 +2098,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="120" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="120" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>55</v>
       </c>
@@ -2139,7 +2134,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>243</v>
       </c>
@@ -2175,7 +2170,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>264</v>
       </c>
@@ -2211,7 +2206,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>67</v>
       </c>
@@ -2247,7 +2242,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>72</v>
       </c>
@@ -2285,7 +2280,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>306</v>
       </c>
@@ -2321,7 +2316,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="84" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="84" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>82</v>
       </c>
@@ -2359,7 +2354,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>88</v>
       </c>
@@ -2397,7 +2392,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>78</v>
       </c>
@@ -2435,7 +2430,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>91</v>
       </c>
@@ -2473,7 +2468,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>96</v>
       </c>
@@ -2511,7 +2506,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>236</v>
       </c>
@@ -2667,7 +2662,7 @@
       <c r="I28" s="16"/>
       <c r="J28" s="18"/>
     </row>
-    <row r="29" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>105</v>
       </c>
@@ -2766,7 +2761,7 @@
       <c r="I31" s="16"/>
       <c r="J31" s="18"/>
     </row>
-    <row r="32" spans="1:12" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>261</v>
       </c>
@@ -2802,7 +2797,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>314</v>
       </c>
@@ -2869,7 +2864,7 @@
       </c>
       <c r="K34" s="15"/>
     </row>
-    <row r="35" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="72" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>118</v>
       </c>
@@ -2933,7 +2928,7 @@
         <v>20</v>
       </c>
       <c r="I36" s="16" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="J36" s="18" t="s">
         <v>47</v>
@@ -2941,8 +2936,11 @@
       <c r="K36" s="18" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="36" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L36" s="18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>62</v>
       </c>
@@ -3011,7 +3009,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="108" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="108" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>126</v>
       </c>
@@ -5304,11 +5302,7 @@
       <c r="J227" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L39" xr:uid="{B3F1C4F4-92F8-4D45-9CD2-F8D7A5E8BEF7}">
-    <filterColumn colId="11">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L39" xr:uid="{B3F1C4F4-92F8-4D45-9CD2-F8D7A5E8BEF7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L39">
     <sortCondition ref="B2:B39"/>
   </sortState>

</xml_diff>